<commit_message>
Se agregan PM codensa a formato phpWord en lib. Formatos
</commit_message>
<xml_diff>
--- a/KANBAN proyecto CASAI.xlsx
+++ b/KANBAN proyecto CASAI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="9435" windowHeight="4530"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="9435" windowHeight="4530"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>PENDIENTES</t>
   </si>
@@ -99,13 +99,19 @@
   </si>
   <si>
     <t>Verificar y modificar codigo phpExcel para generar archivo excel de ot, según requerimiento cliente.</t>
+  </si>
+  <si>
+    <t>Mostrar actividades al editar labor presupuesto.</t>
+  </si>
+  <si>
+    <t>Organizar y mostar phpWord de acuerdo con el formato requerido</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +161,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -219,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -259,6 +272,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -267,7 +283,68 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -543,14 +620,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -562,21 +638,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
     </row>
     <row r="4" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -596,148 +672,150 @@
       </c>
       <c r="C5" s="12"/>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="5"/>
       <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="5"/>
       <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="5"/>
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="5"/>
       <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="5"/>
       <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="5"/>
       <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="5" t="s">
+    <row r="15" spans="1:3" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="5"/>
       <c r="C17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+    </row>
+    <row r="20" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="5"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
-      <c r="B23" s="5"/>
       <c r="C23" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" s="14"/>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+      <c r="A25" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="B25" s="5"/>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
@@ -1115,16 +1193,25 @@
       <c r="C101" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:C24">
-    <filterColumn colId="1">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A4:C24"/>
   <mergeCells count="1">
     <mergeCell ref="A1:C3"/>
   </mergeCells>
+  <conditionalFormatting sqref="A5:A1048576">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:B1048576">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23:C1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Se crean intup en formEditPresup.php, para mostar los valores de % por ubicación y pago a 90 días
</commit_message>
<xml_diff>
--- a/KANBAN proyecto CASAI.xlsx
+++ b/KANBAN proyecto CASAI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="9435" windowHeight="4530"/>
+    <workbookView xWindow="6510" yWindow="0" windowWidth="9435" windowHeight="4530"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>PENDIENTES</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Agregar los PM codensa al formato de ot en phpWord</t>
   </si>
   <si>
-    <t>Sumar automáticamente el valor del 1,25 por pago a 90 días al costo total del presupuesto</t>
-  </si>
-  <si>
     <t>Crear un checkbox que permita seleccionar si la subestacion esta fuera de la ciudad, para asi sumar el 3% al valor total del presupuesto.</t>
   </si>
   <si>
@@ -105,6 +102,15 @@
   </si>
   <si>
     <t>Organizar y mostar phpWord de acuerdo con el formato requerido</t>
+  </si>
+  <si>
+    <t>Mostrar lista de módulos en configuración</t>
+  </si>
+  <si>
+    <t>Sumar automáticamente el valor del 1,5 por pago a 90 días al costo total del presupuesto</t>
+  </si>
+  <si>
+    <t>Solucionar la suma de los valores en phpWord</t>
   </si>
 </sst>
 </file>
@@ -283,7 +289,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF00B050"/>
@@ -292,51 +298,6 @@
     <dxf>
       <font>
         <color rgb="FF002060"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
       </font>
     </dxf>
     <dxf>
@@ -623,10 +584,10 @@
   <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -668,7 +629,7 @@
     <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="12"/>
     </row>
@@ -770,61 +731,64 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="A20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="5"/>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="B22" s="14"/>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="C23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
       <c r="B26" s="5"/>
       <c r="C26" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
       <c r="B27" s="5"/>
       <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
-      <c r="B28" s="5"/>
+      <c r="B28" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1197,7 +1161,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:C3"/>
   </mergeCells>
-  <conditionalFormatting sqref="A5:A1048576">
+  <conditionalFormatting sqref="A5:A25 A27:A1048576">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Se cambiar campos en phpWord para que muestre el valor total con incrementos de la ot
</commit_message>
<xml_diff>
--- a/KANBAN proyecto CASAI.xlsx
+++ b/KANBAN proyecto CASAI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="0" windowWidth="9435" windowHeight="4530"/>
+    <workbookView xWindow="7440" yWindow="0" windowWidth="9435" windowHeight="4530"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Acenergy</author>
+  </authors>
+  <commentList>
+    <comment ref="C18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Acenergy:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Se da por terminada, ya que phpWord no permite darle formato a los arreglos.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
@@ -117,7 +151,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +208,26 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -238,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -284,6 +338,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,21 +637,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.85546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="65.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="56.85546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="61.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="61.5703125" style="3" customWidth="1"/>
     <col min="4" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -716,12 +773,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+    <row r="18" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
@@ -749,7 +806,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="14"/>
-      <c r="C22" s="2"/>
+      <c r="C22" s="16"/>
     </row>
     <row r="23" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
@@ -786,10 +843,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="14"/>
+      <c r="C28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
@@ -1178,5 +1235,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega codigo para que solo muestre inputs de incrementos en editar presupuesto, no al generarlo
</commit_message>
<xml_diff>
--- a/KANBAN proyecto CASAI.xlsx
+++ b/KANBAN proyecto CASAI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="0" windowWidth="9435" windowHeight="4530"/>
+    <workbookView xWindow="9300" yWindow="0" windowWidth="9435" windowHeight="4530"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>PENDIENTES</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>Solucionar la suma de los valores en phpWord</t>
+  </si>
+  <si>
+    <t>Solucionar valor porcentajes en valores totales phpExcel presupuesto</t>
+  </si>
+  <si>
+    <t>Mostrar porcentajes fijos en phpWord</t>
+  </si>
+  <si>
+    <t>Mostar inputs al editar los presupuestos, no al generar</t>
   </si>
 </sst>
 </file>
@@ -336,11 +345,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -641,10 +650,10 @@
   <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -656,21 +665,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
     </row>
     <row r="4" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -788,17 +797,17 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="5"/>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="8"/>
+      <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="5"/>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
@@ -806,7 +815,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="14"/>
-      <c r="C22" s="16"/>
+      <c r="C22" s="15"/>
     </row>
     <row r="23" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
@@ -848,20 +857,26 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="2"/>
+      <c r="B29" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="15"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="5"/>
-      <c r="C30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="5"/>
-      <c r="C31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>

</xml_diff>

<commit_message>
Se modifico en wordOT.php para separa las labores con el mismo modulo y se soluciona los campos donde se muestran los numeros de labores
</commit_message>
<xml_diff>
--- a/KANBAN proyecto CASAI.xlsx
+++ b/KANBAN proyecto CASAI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="0" windowWidth="9435" windowHeight="4530"/>
+    <workbookView xWindow="10230" yWindow="0" windowWidth="9435" windowHeight="4530"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -126,9 +126,6 @@
     <t>Se soluciona problema de inserción de módulo, al cargar una nueva actividad, en editar presupuesto.</t>
   </si>
   <si>
-    <t>Realizar la creación de la documentación base del desarrollo web CASAI</t>
-  </si>
-  <si>
     <t>Verificar y modificar codigo phpExcel para generar archivo excel de ot, según requerimiento cliente.</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>Mostar inputs al editar los presupuestos, no al generar</t>
+  </si>
+  <si>
+    <t>Realizar la creación de la documentación base del desarrollo web CASAI, los viernes.</t>
   </si>
 </sst>
 </file>
@@ -653,7 +653,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -695,7 +695,7 @@
     <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="4" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C5" s="12"/>
     </row>
@@ -782,7 +782,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="5"/>
       <c r="C18" s="2" t="s">
@@ -799,7 +799,7 @@
     <row r="20" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="2"/>
     </row>
@@ -825,27 +825,27 @@
     </row>
     <row r="24" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="2"/>
@@ -854,28 +854,28 @@
       <c r="A28" s="8"/>
       <c r="B28" s="14"/>
       <c r="C28" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
-      <c r="B29" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="15"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="5"/>
       <c r="C30" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="5"/>
       <c r="C31" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se arreglan celdas y datos de labores, cantidad, vr. unitario, total
</commit_message>
<xml_diff>
--- a/KANBAN proyecto CASAI.xlsx
+++ b/KANBAN proyecto CASAI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10230" yWindow="0" windowWidth="9435" windowHeight="4530"/>
+    <workbookView xWindow="11160" yWindow="0" windowWidth="9435" windowHeight="4530"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -56,12 +56,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="B20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Acenergy:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Se detiene desarrollo, para solucionar problemas en phpWord y phpExcel, los cuales generan los documentos del presupuesto</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>PENDIENTES</t>
   </si>
@@ -154,6 +178,12 @@
   </si>
   <si>
     <t>Realizar la creación de la documentación base del desarrollo web CASAI, los viernes.</t>
+  </si>
+  <si>
+    <t>Borrar fila vacia en phpExcel presupuesto</t>
+  </si>
+  <si>
+    <t>Borrar fila repetidas en la tabla de las labores iguales phpWord presupuesto</t>
   </si>
 </sst>
 </file>
@@ -650,10 +680,10 @@
   <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -878,14 +908,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
-      <c r="B32" s="5"/>
+      <c r="B32" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
-      <c r="B33" s="5"/>
+      <c r="B33" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se guardan documentos de presupuesto en su carpeta y en BD, se muestran para descargar
</commit_message>
<xml_diff>
--- a/KANBAN proyecto CASAI.xlsx
+++ b/KANBAN proyecto CASAI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dv_casai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\casai\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>PENDIENTES</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Guardar informacion de archivos presupuestos en base de datos y mostrarlos al subir</t>
+  </si>
+  <si>
+    <t>Permitir eliminar y descargar documentos guardados en carpetas presupuesto</t>
   </si>
 </sst>
 </file>
@@ -605,10 +608,10 @@
   <dimension ref="A1:C99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -856,14 +859,16 @@
     </row>
     <row r="35" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="5"/>
+      <c r="C35" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
-      <c r="B36" s="14"/>
+      <c r="B36" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se crean funciones para eliminar y descargar archivos de presupuesto
</commit_message>
<xml_diff>
--- a/KANBAN proyecto CASAI.xlsx
+++ b/KANBAN proyecto CASAI.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>PENDIENTES</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>Permitir eliminar y descargar documentos guardados en carpetas presupuesto</t>
+  </si>
+  <si>
+    <t>Ajustar php word con los nuevos parametros de incrementos automaticos</t>
   </si>
 </sst>
 </file>
@@ -608,10 +611,10 @@
   <dimension ref="A1:C99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomRight" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -866,19 +869,21 @@
     </row>
     <row r="36" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="5"/>
+      <c r="C36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
-      <c r="B37" s="5"/>
+      <c r="B37" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="C37" s="2"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
-      <c r="B38" s="5"/>
+      <c r="B38" s="14"/>
       <c r="C38" s="2"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cambio menu color azul
</commit_message>
<xml_diff>
--- a/KANBAN proyecto CASAI.xlsx
+++ b/KANBAN proyecto CASAI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13020" yWindow="0" windowWidth="9435" windowHeight="4530"/>
+    <workbookView xWindow="13020" yWindow="450" windowWidth="9435" windowHeight="4530"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>PENDIENTES</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>generar dialogo que solicite número de ot para aprobar presupuesto</t>
+  </si>
+  <si>
+    <t>maquetear el proyecto parte visual</t>
+  </si>
+  <si>
+    <t>solucionar conflictos excel facturación</t>
   </si>
 </sst>
 </file>
@@ -614,10 +620,10 @@
   <dimension ref="A1:C99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A39" sqref="A39"/>
+      <selection pane="bottomRight" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -878,10 +884,10 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="5" t="s">
+      <c r="A37" s="8" t="s">
         <v>36</v>
       </c>
+      <c r="B37" s="5"/>
       <c r="C37" s="2"/>
     </row>
     <row r="38" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
@@ -893,11 +899,15 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
-      <c r="B39" s="5"/>
+      <c r="B39" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="C39" s="2"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
+      <c r="A40" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="B40" s="5"/>
       <c r="C40" s="2"/>
     </row>

</xml_diff>

<commit_message>
se arregla consulta para mostar campo de avance actividad
</commit_message>
<xml_diff>
--- a/KANBAN proyecto CASAI.xlsx
+++ b/KANBAN proyecto CASAI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13020" yWindow="450" windowWidth="9435" windowHeight="4530"/>
+    <workbookView xWindow="13020" yWindow="960" windowWidth="9435" windowHeight="4530"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -146,7 +146,7 @@
     <t>maquetear el proyecto parte visual</t>
   </si>
   <si>
-    <t>solucionar conflictos excel facturación</t>
+    <t>Ajustar excel conciliacion para hacer calculos</t>
   </si>
 </sst>
 </file>
@@ -623,7 +623,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A41" sqref="A41"/>
+      <selection pane="bottomRight" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -905,11 +905,11 @@
       <c r="C39" s="2"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="8"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="2"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>

</xml_diff>

<commit_message>
se cambia el menu principal a diseño aprobado
</commit_message>
<xml_diff>
--- a/KANBAN proyecto CASAI.xlsx
+++ b/KANBAN proyecto CASAI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13020" yWindow="960" windowWidth="9435" windowHeight="4530"/>
+    <workbookView xWindow="13020" yWindow="1410" windowWidth="9435" windowHeight="4530"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>PENDIENTES</t>
   </si>
@@ -143,10 +143,13 @@
     <t>generar dialogo que solicite número de ot para aprobar presupuesto</t>
   </si>
   <si>
-    <t>maquetear el proyecto parte visual</t>
-  </si>
-  <si>
     <t>Ajustar excel conciliacion para hacer calculos</t>
+  </si>
+  <si>
+    <t>maquetear el proyecto parte presupuesto</t>
+  </si>
+  <si>
+    <t>Modificar generacion de presuúesto sin desplazamiento hacia abajo</t>
   </si>
 </sst>
 </file>
@@ -623,7 +626,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C40" sqref="C40"/>
+      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -899,21 +902,23 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
-      <c r="B39" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C39" s="2"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="5"/>
       <c r="C40" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
-      <c r="B41" s="5"/>
+      <c r="B41" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="C41" s="2"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se modifica codigo phpExcel para exportar consolidado de ot, para que llave los datos desde la bd en el resumen(pte 2 pesos de más
</commit_message>
<xml_diff>
--- a/KANBAN proyecto CASAI.xlsx
+++ b/KANBAN proyecto CASAI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13020" yWindow="1410" windowWidth="9435" windowHeight="4530"/>
+    <workbookView minimized="1" xWindow="13020" yWindow="1410" windowWidth="9435" windowHeight="4530"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>PENDIENTES</t>
   </si>
@@ -150,13 +150,19 @@
   </si>
   <si>
     <t>Modificar generacion de presuúesto sin desplazamiento hacia abajo</t>
+  </si>
+  <si>
+    <t>Creacion de modulo de planeación "En pausa"</t>
+  </si>
+  <si>
+    <t>Modificar archivo de conciliacion para que muestre el resumen de forma ordenada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +219,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -277,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -323,6 +336,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -626,7 +642,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -916,20 +932,24 @@
     </row>
     <row r="41" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="5"/>
+      <c r="C41" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="2"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
+      <c r="A42" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="B42" s="5"/>
       <c r="C42" s="2"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="2"/>
+      <c r="B43" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="16"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>

</xml_diff>

<commit_message>
se modifica interfaz para que permita consolidar las labores finalizadas, se agregan calculos para que muestre un resumen del valor total del consolidado en la interfaz
</commit_message>
<xml_diff>
--- a/KANBAN proyecto CASAI.xlsx
+++ b/KANBAN proyecto CASAI.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="13020" yWindow="1410" windowWidth="9435" windowHeight="4530"/>
+    <workbookView xWindow="13020" yWindow="1410" windowWidth="9435" windowHeight="4530"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$4:$C$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$4:$C$20</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>PENDIENTES</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Mostar nombre de usuario al ingresar al sistema.</t>
   </si>
   <si>
-    <t>Insertar porcentaje calculado en base de datos para uso en facturación</t>
-  </si>
-  <si>
     <t>METODOLOGIA AGIL KANBAN</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t>Revisar por que el sistema no permite la creación de nuevas subestaciones, desde el select en generar presupuesto</t>
   </si>
   <si>
-    <t>El sistema debe cambiar los costos de los presupuestos, cuando el usuario seleccione el ultimo contrato creado.</t>
-  </si>
-  <si>
     <t>Realizar cambio en phpWord para que cuando se genere la ot, muestre tildes y espacios donde se solicito</t>
   </si>
   <si>
@@ -149,13 +143,22 @@
     <t>maquetear el proyecto parte presupuesto</t>
   </si>
   <si>
-    <t>Modificar generacion de presuúesto sin desplazamiento hacia abajo</t>
-  </si>
-  <si>
     <t>Creacion de modulo de planeación "En pausa"</t>
   </si>
   <si>
     <t>Modificar archivo de conciliacion para que muestre el resumen de forma ordenada</t>
+  </si>
+  <si>
+    <t>Modificar generacion de presupuesto sin desplazamiento hacia abajo</t>
+  </si>
+  <si>
+    <t>Mostrar valores en la interfaz del usuario de los valores a conciliar de las ot</t>
+  </si>
+  <si>
+    <t>Modificar diseño para que permita consolidar independientemente cada una de las labores realizadas en el mes</t>
+  </si>
+  <si>
+    <t>Modificar codigo, ya que el aplicativo no carga las actas en el archivo excel de conciliación</t>
   </si>
 </sst>
 </file>
@@ -334,11 +337,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,13 +639,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C99"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
+      <selection pane="bottomRight" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -654,21 +657,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="A1" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
     </row>
     <row r="4" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -684,7 +687,7 @@
     <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="12"/>
     </row>
@@ -702,18 +705,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
-      <c r="B9" s="14"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
@@ -727,238 +730,240 @@
       <c r="A11" s="8"/>
       <c r="B11" s="5"/>
       <c r="C11" s="2" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="5"/>
       <c r="C12" s="2" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
-      <c r="B13" s="5"/>
       <c r="C13" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="5"/>
       <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:3" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
       <c r="B16" s="5"/>
       <c r="C16" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="5"/>
       <c r="C17" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="5"/>
       <c r="C18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
-      <c r="B19" s="5"/>
       <c r="C19" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="42.75" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
-      <c r="B20" s="5"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
+      <c r="B21" s="5"/>
       <c r="C21" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="14"/>
+      <c r="B22" s="5"/>
       <c r="C22" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="A23" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="B23" s="5"/>
-      <c r="C23" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="14"/>
       <c r="C24" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="2"/>
+    </row>
+    <row r="25" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
-      <c r="B26" s="14"/>
+      <c r="B26" s="5"/>
       <c r="C26" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
-      <c r="B27" s="14"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
+    <row r="28" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="B28" s="5"/>
-      <c r="C28" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="5"/>
       <c r="C29" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="5"/>
       <c r="C31" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="14"/>
       <c r="C32" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="5"/>
       <c r="C33" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
-      <c r="B34" s="14"/>
+      <c r="B34" s="5"/>
       <c r="C34" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
+      <c r="A35" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="B35" s="5"/>
-      <c r="C35" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="C35" s="2"/>
     </row>
     <row r="36" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="2" t="s">
+      <c r="A36" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+      <c r="B36" s="14"/>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="8"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="2"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="5"/>
       <c r="C39" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
+      <c r="A40" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="B40" s="5"/>
-      <c r="C40" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="5"/>
-      <c r="C41" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" s="5"/>
+      <c r="C41" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="B42" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="C42" s="2"/>
     </row>
     <row r="43" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
-      <c r="B43" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" s="16"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="14"/>
+      <c r="C43" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="5"/>
-      <c r="C44" s="2"/>
+      <c r="C44" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
-      <c r="B45" s="5"/>
+      <c r="B45" s="14"/>
       <c r="C45" s="2"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1221,22 +1226,12 @@
       <c r="B97" s="5"/>
       <c r="C97" s="2"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="8"/>
-      <c r="B98" s="5"/>
-      <c r="C98" s="2"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="8"/>
-      <c r="B99" s="5"/>
-      <c r="C99" s="2"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A4:C22"/>
+  <autoFilter ref="A4:C20"/>
   <mergeCells count="1">
     <mergeCell ref="A1:C3"/>
   </mergeCells>
-  <conditionalFormatting sqref="A25:A1048576 A5:A23">
+  <conditionalFormatting sqref="A23:A1048576 A5:A21">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -1246,7 +1241,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:C1048576">
+  <conditionalFormatting sqref="C19:C1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>